<commit_message>
Code refactoring and new comments
</commit_message>
<xml_diff>
--- a/GETComp/WO2BIGGEST.xlsx
+++ b/GETComp/WO2BIGGEST.xlsx
@@ -17,13 +17,14 @@
     <sheet name="semDoisMaisImportantes" sheetId="3" r:id="rId3"/>
     <sheet name="matriz" sheetId="4" r:id="rId4"/>
     <sheet name="Plan4" sheetId="5" r:id="rId5"/>
+    <sheet name="Plan1" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1004" uniqueCount="129">
   <si>
     <t xml:space="preserve"> 859 27461 49645 50441 62709 66789 97337 99460 99567 116493 122331 123515 130535 148137 265427 </t>
   </si>
@@ -405,12 +406,18 @@
   <si>
     <t>RCLOSENESS x RADIAL</t>
   </si>
+  <si>
+    <t>Semelhança</t>
+  </si>
+  <si>
+    <t>Máximo de informação 15, corte de informação 0.001, desconsiderando interseção, comparação de indivíduos alcançados</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -541,6 +548,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -925,7 +940,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -968,8 +983,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1005,6 +1021,36 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="10" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="18" fillId="0" borderId="10" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1028,14 +1074,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Ênfase1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Ênfase2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Ênfase3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1069,6 +1115,7 @@
     <cellStyle name="Neutra" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Nota" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Porcentagem" xfId="42" builtinId="5"/>
     <cellStyle name="Saída" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Texto de Aviso" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Texto Explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
@@ -13958,24 +14005,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14" t="s">
+      <c r="C2" s="24"/>
+      <c r="D2" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="E2" s="14"/>
+      <c r="E2" s="24"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
@@ -14134,24 +14181,24 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="18"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="28"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14" t="s">
+      <c r="C12" s="24"/>
+      <c r="D12" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="E12" s="14"/>
+      <c r="E12" s="24"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
@@ -16816,55 +16863,55 @@
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" style="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" style="22" customWidth="1"/>
-    <col min="3" max="3" width="8" style="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="22" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" style="22" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" style="22" customWidth="1"/>
-    <col min="7" max="7" width="12" style="22" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" style="22" customWidth="1"/>
-    <col min="9" max="9" width="8.85546875" style="22" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" style="22" customWidth="1"/>
-    <col min="11" max="11" width="9.5703125" style="22" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" style="22" customWidth="1"/>
-    <col min="13" max="13" width="12" style="22" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.85546875" style="22" customWidth="1"/>
-    <col min="15" max="15" width="13" style="22" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="22"/>
+    <col min="1" max="1" width="12" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="15" customWidth="1"/>
+    <col min="3" max="3" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="15" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="15" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" style="15" customWidth="1"/>
+    <col min="7" max="7" width="12" style="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" style="15" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" style="15" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" style="15" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" style="15" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" style="15" customWidth="1"/>
+    <col min="13" max="13" width="12" style="15" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" style="15" customWidth="1"/>
+    <col min="15" max="15" width="13" style="15" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19" t="s">
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="20" t="s">
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21" t="s">
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
@@ -16914,31 +16961,31 @@
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19" t="s">
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19" t="s">
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19" t="s">
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="19" t="s">
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="N3" s="19"/>
-      <c r="O3" s="19"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
@@ -17035,29 +17082,29 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19" t="s">
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19" t="s">
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19" t="s">
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="29"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="16" t="s">
         <v>86</v>
       </c>
       <c r="B7" s="13">
@@ -17095,7 +17142,7 @@
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="16" t="s">
         <v>87</v>
       </c>
       <c r="B8" s="13">
@@ -17133,24 +17180,24 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19" t="s">
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19" t="s">
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="16" t="s">
         <v>86</v>
       </c>
       <c r="B10" s="13">
@@ -17179,7 +17226,7 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="16" t="s">
         <v>88</v>
       </c>
       <c r="B11" s="13">
@@ -17208,19 +17255,19 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19" t="s">
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="23" t="s">
+      <c r="A13" s="16" t="s">
         <v>86</v>
       </c>
       <c r="B13" s="13">
@@ -17240,7 +17287,7 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="16" t="s">
         <v>89</v>
       </c>
       <c r="B14" s="13">
@@ -17260,14 +17307,14 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="16" t="s">
         <v>86</v>
       </c>
       <c r="B16" s="13">
@@ -17278,7 +17325,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="23" t="s">
+      <c r="A17" s="16" t="s">
         <v>91</v>
       </c>
       <c r="B17" s="13">
@@ -17290,6 +17337,8 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D12:F12"/>
     <mergeCell ref="M1:O1"/>
     <mergeCell ref="M3:O3"/>
     <mergeCell ref="A12:C12"/>
@@ -17308,9 +17357,456 @@
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="D3:F3"/>
     <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="D12:F12"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="F2" s="29"/>
+      <c r="G2" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="J2" s="31"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="H4" s="29"/>
+      <c r="I4" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="J4" s="32"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="17">
+        <v>0.404754</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" s="17">
+        <v>0.116603</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="F5" s="17">
+        <v>0.57894599999999996</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H5" s="17">
+        <v>0.52710100000000004</v>
+      </c>
+      <c r="I5" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="J5" s="19">
+        <v>0.58366499999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" s="17">
+        <v>0.56125199999999997</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="D6" s="17">
+        <v>6.1401400000000002E-2</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6" s="17">
+        <v>0.53372200000000003</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="H6" s="17">
+        <v>0.58394000000000001</v>
+      </c>
+      <c r="I6" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="J6" s="21">
+        <v>9.9841899999999997E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="F7" s="29"/>
+      <c r="G7" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="H7" s="32"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" s="17">
+        <v>0.38827800000000001</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" s="17">
+        <v>0.58068299999999995</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="F8" s="17">
+        <v>0.52617499999999995</v>
+      </c>
+      <c r="G8" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="H8" s="19">
+        <v>0.56819500000000001</v>
+      </c>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" s="17">
+        <v>0.55952199999999996</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="D9" s="17">
+        <v>0.52251899999999996</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="F9" s="17">
+        <v>0.500166</v>
+      </c>
+      <c r="G9" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="H9" s="21">
+        <v>0.41571799999999998</v>
+      </c>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="D10" s="29"/>
+      <c r="E10" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="F10" s="32"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" s="17">
+        <v>0.550238</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" s="17">
+        <v>0.510154</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="F11" s="19">
+        <v>0.57511500000000004</v>
+      </c>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" s="17">
+        <v>0.54321900000000001</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12" s="17">
+        <v>0.46973399999999998</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="F12" s="21">
+        <v>0.16864799999999999</v>
+      </c>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="B13" s="29"/>
+      <c r="C13" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="D13" s="32"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" s="17">
+        <v>0.50572799999999996</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" s="19">
+        <v>0.58272500000000005</v>
+      </c>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B15" s="17">
+        <v>0.557759</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15" s="21">
+        <v>0.16864799999999999</v>
+      </c>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="B16" s="32"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="B17" s="19">
+        <v>0.55181899999999995</v>
+      </c>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" s="21">
+        <v>0.282744</v>
+      </c>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="21">
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>